<commit_message>
update paper sheet, Aug20_2025
</commit_message>
<xml_diff>
--- a/outputs/kzfp_all_papers_v2.xlsx
+++ b/outputs/kzfp_all_papers_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/users/qwan/paper_draft/KZFP_review/KZFP_papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qwan/githubRepo/KZFP_review/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5AECB7-4820-3F42-BC1C-5653D409CF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209E92FF-77C7-094C-8FE7-C04021F9666E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="500" windowWidth="47200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35280" yWindow="7700" windowWidth="34300" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - kzfp_all_papers" sheetId="1" r:id="rId1"/>
@@ -24639,8 +24639,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A438" sqref="A438"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A107" zoomScale="96" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -31045,7 +31045,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="184" spans="1:11" s="21" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:11" s="21" customFormat="1" ht="147" x14ac:dyDescent="0.15">
       <c r="A184" s="22" t="s">
         <v>736</v>
       </c>
@@ -31115,7 +31115,7 @@
         <v>4097</v>
       </c>
     </row>
-    <row r="186" spans="1:11" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:11" s="21" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A186" s="22" t="s">
         <v>744</v>
       </c>

</xml_diff>